<commit_message>
Update Dnevnik aktivnosti - FITCC.xlsx
</commit_message>
<xml_diff>
--- a/Smart-home-box-by-Hamza/Dnevnik aktivnosti - FITCC.xlsx
+++ b/Smart-home-box-by-Hamza/Dnevnik aktivnosti - FITCC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SmartHomeBoxByHamza\Smart-home-box-by-Hamza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF9E879-F78F-4F3C-802A-0A91E504AE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD02760-30BC-4BC0-B9E9-2880F57A01CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Implementacija slanja JSON objekata na napravljenje endpointove i testiranje komunikacije na frontendu</t>
   </si>
   <si>
-    <t>02.05.2024.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dodavanje senzora light na arduino, izmjene u Arduino IDE, izmjene u Firebase RT DB </t>
   </si>
   <si>
@@ -105,10 +102,25 @@
     <t>Dodavanje koda u Arduino IDE</t>
   </si>
   <si>
-    <t>Testiranje izvrsne i kontrolne strane</t>
-  </si>
-  <si>
-    <t>29.04.2024.</t>
+    <t>04.05.2024.</t>
+  </si>
+  <si>
+    <t>Implementacija mogucnosti dodavanja vise uredjaja - AUTENTIFIKACIJA</t>
+  </si>
+  <si>
+    <t>Korekcija table u sql bazi podataka i real-time bazi podataka na firebase, kreiranje endpintova na Web API (autentifikacija)</t>
+  </si>
+  <si>
+    <t>Frontend implementacija - AUTENTIFIKACIJA</t>
+  </si>
+  <si>
+    <t>05.05.2024.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korekcija komponente Profil u Angular projektu, dodavanje AuthServisa i Login komponente. </t>
+  </si>
+  <si>
+    <t>Izmjene u zaglavljima endpointova i firebase upita u Arduino IDE</t>
   </si>
 </sst>
 </file>
@@ -486,7 +498,7 @@
   <dimension ref="C2:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,7 +573,7 @@
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
@@ -589,7 +601,7 @@
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
@@ -598,7 +610,7 @@
         <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.3">
@@ -606,23 +618,39 @@
         <v>26</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.3">

</xml_diff>